<commit_message>
Basic data structure to create new templates is now working for File and Image
</commit_message>
<xml_diff>
--- a/ImBel UI.xlsx
+++ b/ImBel UI.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="75" windowWidth="36435" windowHeight="21000"/>
+    <workbookView xWindow="360" yWindow="75" windowWidth="36435" windowHeight="21000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="70">
   <si>
     <t>Menu</t>
   </si>
@@ -91,14 +91,157 @@
   </si>
   <si>
     <t>Oval</t>
+  </si>
+  <si>
+    <t>Object</t>
+  </si>
+  <si>
+    <t>Property</t>
+  </si>
+  <si>
+    <t>Delegate</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>File</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Sharpen amount</t>
+  </si>
+  <si>
+    <t>File type</t>
+  </si>
+  <si>
+    <t>Compression</t>
+  </si>
+  <si>
+    <t>Colorspace</t>
+  </si>
+  <si>
+    <t>File location logic</t>
+  </si>
+  <si>
+    <t>Folder name</t>
+  </si>
+  <si>
+    <t>File suffix</t>
+  </si>
+  <si>
+    <t>Overwrite existing files</t>
+  </si>
+  <si>
+    <t>Checkbox</t>
+  </si>
+  <si>
+    <t>Combobox</t>
+  </si>
+  <si>
+    <t>Slider</t>
+  </si>
+  <si>
+    <t>Text and button</t>
+  </si>
+  <si>
+    <t>SubObject</t>
+  </si>
+  <si>
+    <t>Style</t>
+  </si>
+  <si>
+    <t>Opacity</t>
+  </si>
+  <si>
+    <t>Outside shadow</t>
+  </si>
+  <si>
+    <t>Light direction</t>
+  </si>
+  <si>
+    <t>Light angle</t>
+  </si>
+  <si>
+    <t>Inner shadow</t>
+  </si>
+  <si>
+    <t>Blend mode</t>
+  </si>
+  <si>
+    <t>Distance</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Outer glow</t>
+  </si>
+  <si>
+    <t>Fade</t>
+  </si>
+  <si>
+    <t>Inner glow</t>
+  </si>
+  <si>
+    <t>Bevel</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>IndexCode</t>
+  </si>
+  <si>
+    <t>Contour</t>
+  </si>
+  <si>
+    <t>Texture</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Softness</t>
+  </si>
+  <si>
+    <t>Top</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Bottom</t>
+  </si>
+  <si>
+    <t>Tint color</t>
+  </si>
+  <si>
+    <t>Tint opacity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -393,7 +536,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -439,6 +582,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -741,7 +885,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:P33"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
       <selection activeCell="T31" sqref="T31"/>
     </sheetView>
   </sheetViews>
@@ -1349,13 +1493,1093 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C58" sqref="C58"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="39" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" t="str">
+        <f>B2&amp;C2&amp;D2</f>
+        <v>FileWidth</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E61" si="0">B3&amp;C3&amp;D3</f>
+        <v>FileHeight</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>FileSharpen amount</v>
+      </c>
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>FileFile type</v>
+      </c>
+      <c r="F5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>FileCompression</v>
+      </c>
+      <c r="F6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>FileColorspace</v>
+      </c>
+      <c r="F7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v>FileFile location logic</v>
+      </c>
+      <c r="F8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="0"/>
+        <v>FileFolder name</v>
+      </c>
+      <c r="F9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="0"/>
+        <v>FileFile suffix</v>
+      </c>
+      <c r="F10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="0"/>
+        <v>FileOverwrite existing files</v>
+      </c>
+      <c r="F11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="0"/>
+        <v>ImageStyle</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="0"/>
+        <v>ImageLight direction</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="0"/>
+        <v>ImageLight angle</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="0"/>
+        <v>ImageTexture</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="0"/>
+        <v>ImageTint color</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="0"/>
+        <v>ImageTint opacity</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="0"/>
+        <v>ImageOutside shadowOpacity</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="0"/>
+        <v>ImageOutside shadowBlend mode</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="0"/>
+        <v>ImageOutside shadowDistance</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="0"/>
+        <v>ImageOutside shadowColor</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="0"/>
+        <v>ImageInner shadowOpacity</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="0"/>
+        <v>ImageInner shadowBlend mode</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="0"/>
+        <v>ImageInner shadowDistance</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="0"/>
+        <v>ImageInner shadowColor</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="0"/>
+        <v>ImageOuter glowBlend mode</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27">
+        <v>3</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" t="s">
+        <v>45</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="0"/>
+        <v>ImageOuter glowOpacity</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="0"/>
+        <v>ImageOuter glowFade</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" t="s">
+        <v>51</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="0"/>
+        <v>ImageOuter glowDistance</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30">
+        <v>3</v>
+      </c>
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" t="s">
+        <v>50</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="0"/>
+        <v>ImageInner glowBlend mode</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31">
+        <v>3</v>
+      </c>
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" t="s">
+        <v>45</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="0"/>
+        <v>ImageInner glowOpacity</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32">
+        <v>3</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>55</v>
+      </c>
+      <c r="D32" t="s">
+        <v>54</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="0"/>
+        <v>ImageInner glowFade</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33">
+        <v>3</v>
+      </c>
+      <c r="B33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" t="s">
+        <v>51</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="0"/>
+        <v>ImageInner glowDistance</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34">
+        <v>3</v>
+      </c>
+      <c r="B34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" t="s">
+        <v>56</v>
+      </c>
+      <c r="D34" t="s">
+        <v>57</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="0"/>
+        <v>ImageBevelType</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35">
+        <v>3</v>
+      </c>
+      <c r="B35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" t="s">
+        <v>59</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="0"/>
+        <v>ImageBevelContour</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36">
+        <v>3</v>
+      </c>
+      <c r="B36" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" t="s">
+        <v>56</v>
+      </c>
+      <c r="D36" t="s">
+        <v>62</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" si="0"/>
+        <v>ImageBevelSize</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37">
+        <v>3</v>
+      </c>
+      <c r="B37" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" t="s">
+        <v>56</v>
+      </c>
+      <c r="D37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" si="0"/>
+        <v>ImageBevelSoftness</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38">
+        <v>2</v>
+      </c>
+      <c r="B38" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" t="s">
+        <v>64</v>
+      </c>
+      <c r="E38" t="str">
+        <f t="shared" si="0"/>
+        <v>BorderTop</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39">
+        <v>2</v>
+      </c>
+      <c r="B39" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" t="s">
+        <v>65</v>
+      </c>
+      <c r="E39" t="str">
+        <f t="shared" si="0"/>
+        <v>BorderLeft</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40">
+        <v>2</v>
+      </c>
+      <c r="B40" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" t="s">
+        <v>66</v>
+      </c>
+      <c r="E40" t="str">
+        <f t="shared" si="0"/>
+        <v>BorderRight</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41">
+        <v>2</v>
+      </c>
+      <c r="B41" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" t="s">
+        <v>67</v>
+      </c>
+      <c r="E41" t="str">
+        <f t="shared" si="0"/>
+        <v>BorderBottom</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42">
+        <v>3</v>
+      </c>
+      <c r="B42" t="s">
+        <v>18</v>
+      </c>
+      <c r="C42" t="s">
+        <v>46</v>
+      </c>
+      <c r="D42" t="s">
+        <v>45</v>
+      </c>
+      <c r="E42" t="str">
+        <f t="shared" si="0"/>
+        <v>BorderOutside shadowOpacity</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43">
+        <v>3</v>
+      </c>
+      <c r="B43" t="s">
+        <v>18</v>
+      </c>
+      <c r="C43" t="s">
+        <v>46</v>
+      </c>
+      <c r="D43" t="s">
+        <v>50</v>
+      </c>
+      <c r="E43" t="str">
+        <f t="shared" si="0"/>
+        <v>BorderOutside shadowBlend mode</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44">
+        <v>3</v>
+      </c>
+      <c r="B44" t="s">
+        <v>18</v>
+      </c>
+      <c r="C44" t="s">
+        <v>46</v>
+      </c>
+      <c r="D44" t="s">
+        <v>51</v>
+      </c>
+      <c r="E44" t="str">
+        <f t="shared" si="0"/>
+        <v>BorderOutside shadowDistance</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45">
+        <v>3</v>
+      </c>
+      <c r="B45" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" t="s">
+        <v>46</v>
+      </c>
+      <c r="D45" t="s">
+        <v>52</v>
+      </c>
+      <c r="E45" t="str">
+        <f t="shared" si="0"/>
+        <v>BorderOutside shadowColor</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46">
+        <v>3</v>
+      </c>
+      <c r="B46" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" t="s">
+        <v>49</v>
+      </c>
+      <c r="D46" t="s">
+        <v>45</v>
+      </c>
+      <c r="E46" t="str">
+        <f t="shared" si="0"/>
+        <v>BorderInner shadowOpacity</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47">
+        <v>3</v>
+      </c>
+      <c r="B47" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47" t="s">
+        <v>49</v>
+      </c>
+      <c r="D47" t="s">
+        <v>50</v>
+      </c>
+      <c r="E47" t="str">
+        <f t="shared" si="0"/>
+        <v>BorderInner shadowBlend mode</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48">
+        <v>3</v>
+      </c>
+      <c r="B48" t="s">
+        <v>18</v>
+      </c>
+      <c r="C48" t="s">
+        <v>49</v>
+      </c>
+      <c r="D48" t="s">
+        <v>51</v>
+      </c>
+      <c r="E48" t="str">
+        <f t="shared" si="0"/>
+        <v>BorderInner shadowDistance</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49">
+        <v>3</v>
+      </c>
+      <c r="B49" t="s">
+        <v>18</v>
+      </c>
+      <c r="C49" t="s">
+        <v>49</v>
+      </c>
+      <c r="D49" t="s">
+        <v>52</v>
+      </c>
+      <c r="E49" t="str">
+        <f t="shared" si="0"/>
+        <v>BorderInner shadowColor</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50">
+        <v>3</v>
+      </c>
+      <c r="B50" t="s">
+        <v>18</v>
+      </c>
+      <c r="C50" t="s">
+        <v>53</v>
+      </c>
+      <c r="D50" t="s">
+        <v>50</v>
+      </c>
+      <c r="E50" t="str">
+        <f t="shared" si="0"/>
+        <v>BorderOuter glowBlend mode</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51">
+        <v>3</v>
+      </c>
+      <c r="B51" t="s">
+        <v>18</v>
+      </c>
+      <c r="C51" t="s">
+        <v>53</v>
+      </c>
+      <c r="D51" t="s">
+        <v>45</v>
+      </c>
+      <c r="E51" t="str">
+        <f t="shared" si="0"/>
+        <v>BorderOuter glowOpacity</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52">
+        <v>3</v>
+      </c>
+      <c r="B52" t="s">
+        <v>18</v>
+      </c>
+      <c r="C52" t="s">
+        <v>53</v>
+      </c>
+      <c r="D52" t="s">
+        <v>54</v>
+      </c>
+      <c r="E52" t="str">
+        <f t="shared" si="0"/>
+        <v>BorderOuter glowFade</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53">
+        <v>3</v>
+      </c>
+      <c r="B53" t="s">
+        <v>18</v>
+      </c>
+      <c r="C53" t="s">
+        <v>53</v>
+      </c>
+      <c r="D53" t="s">
+        <v>51</v>
+      </c>
+      <c r="E53" t="str">
+        <f t="shared" si="0"/>
+        <v>BorderOuter glowDistance</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54">
+        <v>3</v>
+      </c>
+      <c r="B54" t="s">
+        <v>18</v>
+      </c>
+      <c r="C54" t="s">
+        <v>55</v>
+      </c>
+      <c r="D54" t="s">
+        <v>50</v>
+      </c>
+      <c r="E54" t="str">
+        <f t="shared" si="0"/>
+        <v>BorderInner glowBlend mode</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55">
+        <v>3</v>
+      </c>
+      <c r="B55" t="s">
+        <v>18</v>
+      </c>
+      <c r="C55" t="s">
+        <v>55</v>
+      </c>
+      <c r="D55" t="s">
+        <v>45</v>
+      </c>
+      <c r="E55" t="str">
+        <f t="shared" si="0"/>
+        <v>BorderInner glowOpacity</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56">
+        <v>3</v>
+      </c>
+      <c r="B56" t="s">
+        <v>18</v>
+      </c>
+      <c r="C56" t="s">
+        <v>55</v>
+      </c>
+      <c r="D56" t="s">
+        <v>54</v>
+      </c>
+      <c r="E56" t="str">
+        <f t="shared" si="0"/>
+        <v>BorderInner glowFade</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57">
+        <v>3</v>
+      </c>
+      <c r="B57" t="s">
+        <v>18</v>
+      </c>
+      <c r="C57" t="s">
+        <v>55</v>
+      </c>
+      <c r="D57" t="s">
+        <v>51</v>
+      </c>
+      <c r="E57" t="str">
+        <f t="shared" si="0"/>
+        <v>BorderInner glowDistance</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58">
+        <v>3</v>
+      </c>
+      <c r="B58" t="s">
+        <v>18</v>
+      </c>
+      <c r="C58" t="s">
+        <v>56</v>
+      </c>
+      <c r="D58" t="s">
+        <v>57</v>
+      </c>
+      <c r="E58" t="str">
+        <f t="shared" si="0"/>
+        <v>BorderBevelType</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59">
+        <v>3</v>
+      </c>
+      <c r="B59" t="s">
+        <v>18</v>
+      </c>
+      <c r="C59" t="s">
+        <v>56</v>
+      </c>
+      <c r="D59" t="s">
+        <v>59</v>
+      </c>
+      <c r="E59" t="str">
+        <f t="shared" si="0"/>
+        <v>BorderBevelContour</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60">
+        <v>3</v>
+      </c>
+      <c r="B60" t="s">
+        <v>18</v>
+      </c>
+      <c r="C60" t="s">
+        <v>56</v>
+      </c>
+      <c r="D60" t="s">
+        <v>62</v>
+      </c>
+      <c r="E60" t="str">
+        <f t="shared" si="0"/>
+        <v>BorderBevelSize</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61">
+        <v>3</v>
+      </c>
+      <c r="B61" t="s">
+        <v>18</v>
+      </c>
+      <c r="C61" t="s">
+        <v>56</v>
+      </c>
+      <c r="D61" t="s">
+        <v>63</v>
+      </c>
+      <c r="E61" t="str">
+        <f t="shared" si="0"/>
+        <v>BorderBevelSoftness</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>